<commit_message>
docs(added configuration parameters): added table configurations
</commit_message>
<xml_diff>
--- a/docs/demo_data.xlsx
+++ b/docs/demo_data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jouke/Projects/molgenis-frontend/packages/job-information-dashboard/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE6B63EB-AF8D-6F4A-AE0F-1E23EEDF3E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4F74E3-4F03-1143-A0C6-16EAE4297294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="827" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="827" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
-    <sheet name="packages" sheetId="3" r:id="rId3"/>
-    <sheet name="status_jobs" sheetId="6" r:id="rId4"/>
-    <sheet name="status_overview" sheetId="7" r:id="rId5"/>
-    <sheet name="status_projects" sheetId="8" r:id="rId6"/>
+    <sheet name="status_clusters" sheetId="9" r:id="rId3"/>
+    <sheet name="packages" sheetId="3" r:id="rId4"/>
+    <sheet name="status_jobs" sheetId="6" r:id="rId5"/>
+    <sheet name="status_overview" sheetId="7" r:id="rId6"/>
+    <sheet name="status_projects" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="203">
   <si>
     <t>entity</t>
   </si>
@@ -609,9 +610,6 @@
     <t>statistics_test-2_hasrunspv</t>
   </si>
   <si>
-    <t>aaaac3wwfsa676qwhzjo7ayaae</t>
-  </si>
-  <si>
     <t>cluster_name</t>
   </si>
   <si>
@@ -624,6 +622,9 @@
     <t>Latest Ping</t>
   </si>
   <si>
+    <t>clusters</t>
+  </si>
+  <si>
     <t>Clusters</t>
   </si>
   <si>
@@ -631,6 +632,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Boxy</t>
+  </si>
+  <si>
+    <t>Calculon</t>
+  </si>
+  <si>
+    <t>status_clusters</t>
   </si>
 </sst>
 </file>
@@ -1491,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4214,13 +4224,13 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>202</v>
+      </c>
+      <c r="B70" t="s">
         <v>192</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>193</v>
-      </c>
-      <c r="C70" t="s">
-        <v>194</v>
       </c>
       <c r="D70" t="s">
         <v>42</v>
@@ -4252,13 +4262,13 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" t="s">
         <v>195</v>
-      </c>
-      <c r="C71" t="s">
-        <v>196</v>
       </c>
       <c r="D71" t="s">
         <v>57</v>
@@ -4303,7 +4313,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4454,7 +4464,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
@@ -4477,6 +4487,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AED08A-B233-0E48-A696-EC3CFDD99D8F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4522,12 +4571,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4764,7 +4813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -4837,7 +4886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>

</xml_diff>